<commit_message>
Changed point to time for better graph orientation
</commit_message>
<xml_diff>
--- a/Dashboard Data.xlsx
+++ b/Dashboard Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DR . M ALI MEMON\PycharmProjects\Giraffe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AI &amp; python\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Point</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Voltage</t>
   </si>
@@ -35,64 +32,7 @@
     <t>Current</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>P8</t>
-  </si>
-  <si>
-    <t>P9</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>P11</t>
-  </si>
-  <si>
-    <t>P12</t>
-  </si>
-  <si>
-    <t>P13</t>
-  </si>
-  <si>
-    <t>P14</t>
-  </si>
-  <si>
-    <t>P15</t>
-  </si>
-  <si>
-    <t>P16</t>
-  </si>
-  <si>
-    <t>P17</t>
-  </si>
-  <si>
-    <t>P18</t>
-  </si>
-  <si>
-    <t>P19</t>
-  </si>
-  <si>
-    <t>P20</t>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -480,26 +420,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
+      <c r="A2" s="2">
+        <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
@@ -509,8 +449,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" s="2">
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>9</v>
@@ -520,8 +460,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
+      <c r="A4" s="2">
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>8</v>
@@ -531,7 +471,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="2">
         <v>6</v>
       </c>
       <c r="B5" s="2">
@@ -542,8 +482,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
+      <c r="A6" s="2">
+        <v>9</v>
       </c>
       <c r="B6" s="2">
         <v>8</v>
@@ -553,8 +493,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
+      <c r="A7" s="2">
+        <v>12</v>
       </c>
       <c r="B7" s="2">
         <v>4</v>
@@ -564,8 +504,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
+      <c r="A8" s="2">
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>55</v>
@@ -575,8 +515,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
+      <c r="A9" s="2">
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>50</v>
@@ -586,8 +526,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
+      <c r="A10" s="2">
+        <v>17</v>
       </c>
       <c r="B10" s="2">
         <v>35</v>
@@ -597,8 +537,8 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
+      <c r="A11" s="2">
+        <v>18</v>
       </c>
       <c r="B11" s="2">
         <v>24</v>
@@ -608,8 +548,8 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
+      <c r="A12" s="2">
+        <v>20</v>
       </c>
       <c r="B12" s="2">
         <v>33</v>
@@ -619,8 +559,8 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
+      <c r="A13" s="2">
+        <v>21</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -630,8 +570,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>15</v>
+      <c r="A14" s="3">
+        <v>25</v>
       </c>
       <c r="B14" s="2">
         <v>7</v>
@@ -641,8 +581,8 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>16</v>
+      <c r="A15" s="3">
+        <v>27</v>
       </c>
       <c r="B15" s="2">
         <v>8</v>
@@ -652,8 +592,8 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>17</v>
+      <c r="A16" s="3">
+        <v>28</v>
       </c>
       <c r="B16" s="2">
         <v>4</v>
@@ -663,8 +603,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>18</v>
+      <c r="A17" s="3">
+        <v>30</v>
       </c>
       <c r="B17" s="2">
         <v>55</v>
@@ -674,8 +614,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>19</v>
+      <c r="A18" s="3">
+        <v>31</v>
       </c>
       <c r="B18" s="2">
         <v>50</v>
@@ -685,8 +625,8 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>20</v>
+      <c r="A19" s="3">
+        <v>32</v>
       </c>
       <c r="B19" s="2">
         <v>7</v>
@@ -696,8 +636,8 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>21</v>
+      <c r="A20" s="3">
+        <v>38</v>
       </c>
       <c r="B20" s="2">
         <v>8</v>
@@ -707,8 +647,8 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>22</v>
+      <c r="A21" s="3">
+        <v>40</v>
       </c>
       <c r="B21" s="3">
         <v>23</v>

</xml_diff>